<commit_message>
(ADD) Added 3 eda weasel models, the first is trained on Lior's 1st experiment data the second is trained on Lior's 1st and 2nd experiment data and the third is trained in Lior's 1st and 2nd experiment data and on Vlad's 1st experiment data
</commit_message>
<xml_diff>
--- a/eda_weasel/train_data/EDA_lior_2.xlsx
+++ b/eda_weasel/train_data/EDA_lior_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robo Project\eda_rocket\train_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8D47D2-F441-4DBA-877C-0D0BF2CF5A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C5BEC3-5E05-4534-ABA4-BB68588BC526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFB22E31-E5F5-4E5F-B827-1C54F7BA0498}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{AFB22E31-E5F5-4E5F-B827-1C54F7BA0498}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="4">
   <si>
-    <t>segment id</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Segment id</t>
   </si>
 </sst>
 </file>
@@ -58,14 +58,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -414,397 +414,397 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D0F696-7E6C-4D58-B1F2-4198EA8FD6CE}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.125" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>